<commit_message>
Git Title: systemd template support added
Git Description:
Added support for generating systemd service files
using a specified template.
</commit_message>
<xml_diff>
--- a/machines.xlsx
+++ b/machines.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">192.168.0.140</t>
   </si>
   <si>
-    <t xml:space="preserve">ST1</t>
+    <t xml:space="preserve">st1</t>
   </si>
   <si>
     <t xml:space="preserve">Logger for st2</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">192.168.0.141</t>
   </si>
   <si>
-    <t xml:space="preserve">ST2</t>
+    <t xml:space="preserve">st2</t>
   </si>
   <si>
     <t xml:space="preserve">Logger for st3</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">192.168.0.142</t>
   </si>
   <si>
-    <t xml:space="preserve">ST3</t>
+    <t xml:space="preserve">st3</t>
   </si>
 </sst>
 </file>
@@ -79,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,8 +139,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,80 +274,80 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>5052</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>5053</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5054</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>